<commit_message>
Begin fleshing out actual content
</commit_message>
<xml_diff>
--- a/abilities.xlsx
+++ b/abilities.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Title</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Basic Martial Ability</t>
   </si>
   <si>
-    <t>base.svg</t>
+    <t>gray.svg</t>
   </si>
   <si>
     <t>broadsword.svg</t>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Ranged Weapon Attack</t>
+  </si>
+  <si>
+    <t>brown.svg</t>
   </si>
   <si>
     <t>Ranged</t>
@@ -311,7 +314,7 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -420,7 +423,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>15</v>
@@ -435,7 +438,7 @@
         <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>18</v>
@@ -444,21 +447,21 @@
         <v>2015</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>15</v>
@@ -470,10 +473,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>18</v>
@@ -482,21 +485,21 @@
         <v>2015</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>15</v>
@@ -511,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>18</v>
@@ -520,10 +523,10 @@
         <v>2015</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more items to the pool
</commit_message>
<xml_diff>
--- a/abilities.xlsx
+++ b/abilities.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -53,77 +53,88 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Melee Weapon Attack</t>
-  </si>
-  <si>
-    <t>Basic Martial Ability</t>
-  </si>
-  <si>
-    <t>gray.svg</t>
+    <t>Defensive Fighting</t>
+  </si>
+  <si>
+    <t>Level 1 Martial Ability</t>
+  </si>
+  <si>
+    <t>brown.svg</t>
   </si>
   <si>
     <t>broadsword.svg</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
     <t>×1</t>
   </si>
   <si>
-    <t>Melee, Weapon, Basic</t>
+    <t>Melee, Weapon, Defensive</t>
   </si>
   <si>
     <t>Thane Brimhall</t>
   </si>
   <si>
-    <t>One target within weapon's reach if it's willing or you have a greater attack than it has defense</t>
-  </si>
-  <si>
-    <t>Bacon ipsum dolor amet fatback rump salami picanha, short loin ham hock turducken tongue pig venison pork. Beef ribeye [pastrami andouille]. T-bone jerky boudin ground round tail. Tenderloin turducken tri-tip beef ribs sausage ham doner capicola. Pork loin alcatra fatback sirloin boudin pork belly pig pastrami. Biltong drumstick turkey [venison] corned beef porchetta. Boudin jowl venison bacon, ham pork sausage tenderloin short loin shank biltong.
-Fatback pork chop filet mignon, capicola rump ground round beef ribs. Tongue [prosciutto] sirloin corned beef jerky, hamburger ball tip shankle pork chop picanha salami. Brisket meatloaf swine sausage jowl boudin spare ribs flank chicken pork belly pig bacon frankfurter. Pork tongue cupim fatback flank prosciutto jerky. Ground round ham hock beef ribs biltong porchetta pork doner short ribs ham tenderloin tri-tip pork chop. Biltong ham prosciutto pork chop, pork loin landjaeger chuck rump.</t>
-  </si>
-  <si>
-    <t>Ranged Weapon Attack</t>
-  </si>
-  <si>
-    <t>brown.svg</t>
-  </si>
-  <si>
-    <t>Ranged</t>
-  </si>
-  <si>
-    <t>One target within weapon's range</t>
-  </si>
-  <si>
-    <t>Roll a d20 to hit. Then roll your damage if you did hit.</t>
-  </si>
-  <si>
-    <t>Magic Missile</t>
-  </si>
-  <si>
-    <t>Basic Arcane Ability</t>
-  </si>
-  <si>
-    <t>3d6+1</t>
-  </si>
-  <si>
-    <t>Arcane, Force</t>
-  </si>
-  <si>
-    <t>One target within implement's range</t>
-  </si>
-  <si>
-    <t>Quick Attack</t>
-  </si>
-  <si>
-    <t>Level 1 Martial Ability</t>
-  </si>
-  <si>
-    <t>Melee, Light Weapon</t>
-  </si>
-  <si>
-    <t>One target within weapon's reach</t>
-  </si>
-  <si>
-    <t>Only usable with [light weapon]</t>
+    <t>Weapon's target</t>
+  </si>
+  <si>
+    <t>Make a [MELEE] [WEAPON] attack with a -2 penalty to the attack roll. If you do, you gain a +4 bonus to [DODGE] until your cooldown is over.</t>
+  </si>
+  <si>
+    <t>Flurry</t>
+  </si>
+  <si>
+    <t>Level 3 Martial Ability</t>
+  </si>
+  <si>
+    <t>Melee, Weapon</t>
+  </si>
+  <si>
+    <t>Make a [MELEE] [WEAPON] attack against the target. If it hits, you may reuse this ability against another target adjacent to the previous target in 1 second (rather than the full 6 second cooldown). You must pay the 6 second cooldown if there are no more targets or if you miss. A target cannot be affected by Cleave more than once before paying the full cooldown.</t>
+  </si>
+  <si>
+    <t>Unarmed Strike</t>
+  </si>
+  <si>
+    <t>1d4</t>
+  </si>
+  <si>
+    <t>Melee, Unarmed</t>
+  </si>
+  <si>
+    <t>One adjacent target</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Cleave</t>
+  </si>
+  <si>
+    <t>Level 2 Martial Ability</t>
+  </si>
+  <si>
+    <t>One primary weapon target and a secondary weapon target adjacent to the first.</t>
+  </si>
+  <si>
+    <t>Make a [MELEE] [WEAPON] attack against the primary target. If it hits, also make a [MELEE] [WEAPON] attack against the secondary target.</t>
+  </si>
+  <si>
+    <t>Sneak Attack</t>
+  </si>
+  <si>
+    <t>Level 1 Rogue Ability</t>
+  </si>
+  <si>
+    <t>×1+2d6</t>
+  </si>
+  <si>
+    <t>Weapon's target if the target is flanked, surprised, or unable to defend itself.</t>
+  </si>
+  <si>
+    <t>Make a [MELEE] [WEAPON] attack against the target. If it hits, deal the weapon's damage, plus an additional 2d6 damage of the weapon's type.</t>
   </si>
 </sst>
 </file>
@@ -311,10 +322,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -326,10 +337,10 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.35204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2448979591837"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.6530612244898"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="77.015306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="68.1275510204082"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="117.326530612245"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
   </cols>
@@ -377,7 +388,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -390,64 +401,64 @@
       <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>6</v>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>25</v>
@@ -458,37 +469,37 @@
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="G4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="I4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="K4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,7 +510,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>15</v>
@@ -508,25 +519,63 @@
         <v>0</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>